<commit_message>
create script to create a full list of language attributions
</commit_message>
<xml_diff>
--- a/data-export/WD_BDRC_data_with_langs.xlsx
+++ b/data-export/WD_BDRC_data_with_langs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/data-export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC6EE2A-BECE-1C41-BD37-1677CF08472E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1852B8-12CF-B849-AF97-E277AD51F129}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="30420" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16100" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DergeKangyur" sheetId="1" r:id="rId1"/>
@@ -7649,8 +7649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="M299" sqref="M299"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7800,7 +7800,7 @@
         <v>50</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>